<commit_message>
Update to 0.105.0-rc (#368)
* Update ClosedXML to 0.104.1, test fail

---------

Co-authored-by: Aleksei <pankraty@gmail.com>
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_TotalLabel.xlsx
+++ b/tests/Gauges/GroupTagTests_TotalLabel.xlsx
@@ -437,7 +437,6 @@
       <x:sz val="8"/>
       <x:name val="Arial"/>
       <x:family val="2"/>
-      <x:charset val="204"/>
     </x:font>
     <x:font>
       <x:sz val="9"/>
@@ -485,7 +484,6 @@
       <x:color indexed="9"/>
       <x:name val="Arial"/>
       <x:family val="2"/>
-      <x:charset val="204"/>
     </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
@@ -1417,25 +1415,25 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="C10" s="41">
-        <x:v>1129</x:v>
+        <x:v>1029</x:v>
       </x:c>
       <x:c r="D10" s="40" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="E10" s="42">
-        <x:v>34261</x:v>
+        <x:v>32343</x:v>
       </x:c>
       <x:c r="F10" s="42">
-        <x:v>34261</x:v>
+        <x:v>32342</x:v>
       </x:c>
       <x:c r="G10" s="43">
-        <x:v>1004.8</x:v>
+        <x:v>20108</x:v>
       </x:c>
       <x:c r="H10" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I10" s="43">
-        <x:v>1004.8</x:v>
+        <x:v>20108</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -1443,23 +1441,23 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="C11" s="41">
-        <x:v>1029</x:v>
+        <x:v>1129</x:v>
       </x:c>
       <x:c r="D11" s="40"/>
       <x:c r="E11" s="42">
-        <x:v>32343</x:v>
+        <x:v>34261</x:v>
       </x:c>
       <x:c r="F11" s="42">
-        <x:v>32342</x:v>
+        <x:v>34261</x:v>
       </x:c>
       <x:c r="G11" s="43">
-        <x:v>20108</x:v>
+        <x:v>1004.8</x:v>
       </x:c>
       <x:c r="H11" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I11" s="43">
-        <x:v>20108</x:v>
+        <x:v>1004.8</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:11" ht="10.2" customHeight="1" outlineLevel="2">
@@ -1615,23 +1613,23 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C20" s="41">
-        <x:v>1217</x:v>
+        <x:v>1117</x:v>
       </x:c>
       <x:c r="D20" s="40"/>
       <x:c r="E20" s="42">
-        <x:v>34660</x:v>
+        <x:v>34072</x:v>
       </x:c>
       <x:c r="F20" s="42">
-        <x:v>34660</x:v>
+        <x:v>34072</x:v>
       </x:c>
       <x:c r="G20" s="43">
-        <x:v>51730.8</x:v>
+        <x:v>6734.85</x:v>
       </x:c>
       <x:c r="H20" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I20" s="43">
-        <x:v>51730.8</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -1639,23 +1637,23 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C21" s="41">
-        <x:v>1117</x:v>
+        <x:v>1217</x:v>
       </x:c>
       <x:c r="D21" s="40"/>
       <x:c r="E21" s="42">
-        <x:v>34072</x:v>
+        <x:v>34660</x:v>
       </x:c>
       <x:c r="F21" s="42">
-        <x:v>34072</x:v>
+        <x:v>34660</x:v>
       </x:c>
       <x:c r="G21" s="43">
-        <x:v>6734.85</x:v>
+        <x:v>51730.8</x:v>
       </x:c>
       <x:c r="H21" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I21" s="43">
-        <x:v>0</x:v>
+        <x:v>51730.8</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -1701,25 +1699,25 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C24" s="41">
-        <x:v>1137</x:v>
+        <x:v>1037</x:v>
       </x:c>
       <x:c r="D24" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="42">
-        <x:v>34300</x:v>
+        <x:v>32382</x:v>
       </x:c>
       <x:c r="F24" s="42">
-        <x:v>34300</x:v>
+        <x:v>32381</x:v>
       </x:c>
       <x:c r="G24" s="43">
-        <x:v>6785.4</x:v>
+        <x:v>3117</x:v>
       </x:c>
       <x:c r="H24" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I24" s="43">
-        <x:v>6785.4</x:v>
+        <x:v>3117</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -1727,23 +1725,23 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C25" s="41">
-        <x:v>1037</x:v>
+        <x:v>1099</x:v>
       </x:c>
       <x:c r="D25" s="40"/>
       <x:c r="E25" s="42">
-        <x:v>32382</x:v>
+        <x:v>32675</x:v>
       </x:c>
       <x:c r="F25" s="42">
-        <x:v>32381</x:v>
+        <x:v>32675</x:v>
       </x:c>
       <x:c r="G25" s="43">
-        <x:v>3117</x:v>
+        <x:v>859.95</x:v>
       </x:c>
       <x:c r="H25" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I25" s="43">
-        <x:v>3117</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -1751,23 +1749,23 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C26" s="41">
-        <x:v>1099</x:v>
+        <x:v>1137</x:v>
       </x:c>
       <x:c r="D26" s="40"/>
       <x:c r="E26" s="42">
-        <x:v>32675</x:v>
+        <x:v>34300</x:v>
       </x:c>
       <x:c r="F26" s="42">
-        <x:v>32675</x:v>
+        <x:v>34300</x:v>
       </x:c>
       <x:c r="G26" s="43">
-        <x:v>859.95</x:v>
+        <x:v>6785.4</x:v>
       </x:c>
       <x:c r="H26" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I26" s="43">
-        <x:v>0</x:v>
+        <x:v>6785.4</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:11" ht="10.2" customHeight="1" outlineLevel="2">
@@ -1789,25 +1787,25 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C28" s="41">
-        <x:v>1294</x:v>
+        <x:v>1074</x:v>
       </x:c>
       <x:c r="D28" s="40" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="E28" s="42">
-        <x:v>34703</x:v>
+        <x:v>32618</x:v>
       </x:c>
       <x:c r="F28" s="42">
-        <x:v>34703</x:v>
+        <x:v>32617</x:v>
       </x:c>
       <x:c r="G28" s="43">
-        <x:v>3304.85</x:v>
+        <x:v>2195</x:v>
       </x:c>
       <x:c r="H28" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I28" s="43">
-        <x:v>3304.85</x:v>
+        <x:v>2195</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -1815,23 +1813,23 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C29" s="41">
-        <x:v>1074</x:v>
+        <x:v>1294</x:v>
       </x:c>
       <x:c r="D29" s="40"/>
       <x:c r="E29" s="42">
-        <x:v>32618</x:v>
+        <x:v>34703</x:v>
       </x:c>
       <x:c r="F29" s="42">
-        <x:v>32617</x:v>
+        <x:v>34703</x:v>
       </x:c>
       <x:c r="G29" s="43">
-        <x:v>2195</x:v>
+        <x:v>3304.85</x:v>
       </x:c>
       <x:c r="H29" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I29" s="43">
-        <x:v>2195</x:v>
+        <x:v>3304.85</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:11" ht="10.2" customHeight="1" outlineLevel="1">
@@ -1907,25 +1905,25 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="C34" s="41">
-        <x:v>1355</x:v>
+        <x:v>1263</x:v>
       </x:c>
       <x:c r="D34" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="42">
-        <x:v>34735</x:v>
+        <x:v>34682</x:v>
       </x:c>
       <x:c r="F34" s="42">
-        <x:v>34735</x:v>
+        <x:v>34682</x:v>
       </x:c>
       <x:c r="G34" s="43">
-        <x:v>13908</x:v>
+        <x:v>158922.65</x:v>
       </x:c>
       <x:c r="H34" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I34" s="43">
-        <x:v>13908</x:v>
+        <x:v>158922.65</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -1933,23 +1931,23 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="C35" s="41">
-        <x:v>1263</x:v>
+        <x:v>1355</x:v>
       </x:c>
       <x:c r="D35" s="40"/>
       <x:c r="E35" s="42">
-        <x:v>34682</x:v>
+        <x:v>34735</x:v>
       </x:c>
       <x:c r="F35" s="42">
-        <x:v>34682</x:v>
+        <x:v>34735</x:v>
       </x:c>
       <x:c r="G35" s="43">
-        <x:v>158922.65</x:v>
+        <x:v>13908</x:v>
       </x:c>
       <x:c r="H35" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I35" s="43">
-        <x:v>158922.65</x:v>
+        <x:v>13908</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:11" ht="10.2" customHeight="1" outlineLevel="1">
@@ -2205,25 +2203,25 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="C49" s="41">
-        <x:v>1106</x:v>
+        <x:v>1006</x:v>
       </x:c>
       <x:c r="D49" s="40" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="E49" s="42">
-        <x:v>33870</x:v>
+        <x:v>32454</x:v>
       </x:c>
       <x:c r="F49" s="42">
-        <x:v>33870</x:v>
+        <x:v>34644</x:v>
       </x:c>
       <x:c r="G49" s="43">
-        <x:v>3531.8</x:v>
+        <x:v>31987</x:v>
       </x:c>
       <x:c r="H49" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I49" s="43">
-        <x:v>3531.8</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2231,23 +2229,23 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="C50" s="41">
-        <x:v>1006</x:v>
+        <x:v>1106</x:v>
       </x:c>
       <x:c r="D50" s="40"/>
       <x:c r="E50" s="42">
-        <x:v>32454</x:v>
+        <x:v>33870</x:v>
       </x:c>
       <x:c r="F50" s="42">
-        <x:v>34644</x:v>
+        <x:v>33870</x:v>
       </x:c>
       <x:c r="G50" s="43">
-        <x:v>31987</x:v>
+        <x:v>3531.8</x:v>
       </x:c>
       <x:c r="H50" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I50" s="43">
-        <x:v>0</x:v>
+        <x:v>3531.8</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:11" ht="10.2" customHeight="1" outlineLevel="1">
@@ -2283,25 +2281,25 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C53" s="41">
-        <x:v>1283</x:v>
+        <x:v>1083</x:v>
       </x:c>
       <x:c r="D53" s="40" t="s">
         <x:v>37</x:v>
       </x:c>
       <x:c r="E53" s="42">
-        <x:v>34698</x:v>
+        <x:v>32638</x:v>
       </x:c>
       <x:c r="F53" s="42">
-        <x:v>34698</x:v>
+        <x:v>32637</x:v>
       </x:c>
       <x:c r="G53" s="43">
-        <x:v>7134</x:v>
+        <x:v>11164.8</x:v>
       </x:c>
       <x:c r="H53" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I53" s="43">
-        <x:v>7134</x:v>
+        <x:v>11164.8</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2309,23 +2307,23 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C54" s="41">
-        <x:v>1083</x:v>
+        <x:v>1283</x:v>
       </x:c>
       <x:c r="D54" s="40"/>
       <x:c r="E54" s="42">
-        <x:v>32638</x:v>
+        <x:v>34698</x:v>
       </x:c>
       <x:c r="F54" s="42">
-        <x:v>32637</x:v>
+        <x:v>34698</x:v>
       </x:c>
       <x:c r="G54" s="43">
-        <x:v>11164.8</x:v>
+        <x:v>7134</x:v>
       </x:c>
       <x:c r="H54" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I54" s="43">
-        <x:v>11164.8</x:v>
+        <x:v>7134</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:11" ht="10.2" customHeight="1" outlineLevel="2">
@@ -2347,25 +2345,25 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C56" s="41">
-        <x:v>1061</x:v>
+        <x:v>1012</x:v>
       </x:c>
       <x:c r="D56" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E56" s="42">
-        <x:v>32571</x:v>
+        <x:v>32283</x:v>
       </x:c>
       <x:c r="F56" s="42">
-        <x:v>32570</x:v>
+        <x:v>32282</x:v>
       </x:c>
       <x:c r="G56" s="43">
-        <x:v>24277.3</x:v>
+        <x:v>5201</x:v>
       </x:c>
       <x:c r="H56" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I56" s="43">
-        <x:v>24277.3</x:v>
+        <x:v>5201</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2397,23 +2395,23 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C58" s="41">
-        <x:v>1212</x:v>
+        <x:v>1061</x:v>
       </x:c>
       <x:c r="D58" s="40"/>
       <x:c r="E58" s="42">
-        <x:v>34652</x:v>
+        <x:v>32571</x:v>
       </x:c>
       <x:c r="F58" s="42">
-        <x:v>34652</x:v>
+        <x:v>32570</x:v>
       </x:c>
       <x:c r="G58" s="43">
-        <x:v>3975.75</x:v>
+        <x:v>24277.3</x:v>
       </x:c>
       <x:c r="H58" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I58" s="43">
-        <x:v>3975.75</x:v>
+        <x:v>24277.3</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2445,23 +2443,23 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C60" s="41">
-        <x:v>1261</x:v>
+        <x:v>1161</x:v>
       </x:c>
       <x:c r="D60" s="40"/>
       <x:c r="E60" s="42">
-        <x:v>34679</x:v>
+        <x:v>34489</x:v>
       </x:c>
       <x:c r="F60" s="42">
-        <x:v>34679</x:v>
+        <x:v>34489</x:v>
       </x:c>
       <x:c r="G60" s="43">
-        <x:v>1999</x:v>
+        <x:v>102453.6</x:v>
       </x:c>
       <x:c r="H60" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I60" s="43">
-        <x:v>1999</x:v>
+        <x:v>102453.6</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2469,23 +2467,23 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C61" s="41">
-        <x:v>1012</x:v>
+        <x:v>1212</x:v>
       </x:c>
       <x:c r="D61" s="40"/>
       <x:c r="E61" s="42">
-        <x:v>32283</x:v>
+        <x:v>34652</x:v>
       </x:c>
       <x:c r="F61" s="42">
-        <x:v>32282</x:v>
+        <x:v>34652</x:v>
       </x:c>
       <x:c r="G61" s="43">
-        <x:v>5201</x:v>
+        <x:v>3975.75</x:v>
       </x:c>
       <x:c r="H61" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I61" s="43">
-        <x:v>5201</x:v>
+        <x:v>3975.75</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2493,23 +2491,23 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C62" s="41">
-        <x:v>1161</x:v>
+        <x:v>1261</x:v>
       </x:c>
       <x:c r="D62" s="40"/>
       <x:c r="E62" s="42">
-        <x:v>34489</x:v>
+        <x:v>34679</x:v>
       </x:c>
       <x:c r="F62" s="42">
-        <x:v>34489</x:v>
+        <x:v>34679</x:v>
       </x:c>
       <x:c r="G62" s="43">
-        <x:v>102453.6</x:v>
+        <x:v>1999</x:v>
       </x:c>
       <x:c r="H62" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I62" s="43">
-        <x:v>102453.6</x:v>
+        <x:v>1999</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:11" ht="10.2" customHeight="1" outlineLevel="2">
@@ -2689,25 +2687,25 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C72" s="41">
-        <x:v>1162</x:v>
+        <x:v>1031</x:v>
       </x:c>
       <x:c r="D72" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E72" s="42">
-        <x:v>34494</x:v>
+        <x:v>32356</x:v>
       </x:c>
       <x:c r="F72" s="42">
-        <x:v>34494</x:v>
+        <x:v>32352</x:v>
       </x:c>
       <x:c r="G72" s="43">
-        <x:v>3153</x:v>
+        <x:v>12685</x:v>
       </x:c>
       <x:c r="H72" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I72" s="43">
-        <x:v>3153</x:v>
+        <x:v>12685</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2715,23 +2713,23 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C73" s="41">
-        <x:v>1031</x:v>
+        <x:v>1058</x:v>
       </x:c>
       <x:c r="D73" s="40"/>
       <x:c r="E73" s="42">
-        <x:v>32356</x:v>
+        <x:v>32561</x:v>
       </x:c>
       <x:c r="F73" s="42">
-        <x:v>32352</x:v>
+        <x:v>32560</x:v>
       </x:c>
       <x:c r="G73" s="43">
-        <x:v>12685</x:v>
+        <x:v>12736</x:v>
       </x:c>
       <x:c r="H73" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I73" s="43">
-        <x:v>12685</x:v>
+        <x:v>12736</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2739,23 +2737,23 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C74" s="41">
-        <x:v>1064</x:v>
+        <x:v>1062</x:v>
       </x:c>
       <x:c r="D74" s="40"/>
       <x:c r="E74" s="42">
-        <x:v>32592</x:v>
+        <x:v>32576</x:v>
       </x:c>
       <x:c r="F74" s="42">
-        <x:v>32591</x:v>
+        <x:v>32575</x:v>
       </x:c>
       <x:c r="G74" s="43">
-        <x:v>395</x:v>
+        <x:v>18320</x:v>
       </x:c>
       <x:c r="H74" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I74" s="43">
-        <x:v>395</x:v>
+        <x:v>18320</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2763,23 +2761,23 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C75" s="41">
-        <x:v>1131</x:v>
+        <x:v>1064</x:v>
       </x:c>
       <x:c r="D75" s="40"/>
       <x:c r="E75" s="42">
-        <x:v>34274</x:v>
+        <x:v>32592</x:v>
       </x:c>
       <x:c r="F75" s="42">
-        <x:v>34274</x:v>
+        <x:v>32591</x:v>
       </x:c>
       <x:c r="G75" s="43">
-        <x:v>11989.2</x:v>
+        <x:v>395</x:v>
       </x:c>
       <x:c r="H75" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I75" s="43">
-        <x:v>11989.2</x:v>
+        <x:v>395</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2787,23 +2785,23 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C76" s="41">
-        <x:v>1058</x:v>
+        <x:v>1131</x:v>
       </x:c>
       <x:c r="D76" s="40"/>
       <x:c r="E76" s="42">
-        <x:v>32561</x:v>
+        <x:v>34274</x:v>
       </x:c>
       <x:c r="F76" s="42">
-        <x:v>32560</x:v>
+        <x:v>34274</x:v>
       </x:c>
       <x:c r="G76" s="43">
-        <x:v>12736</x:v>
+        <x:v>11989.2</x:v>
       </x:c>
       <x:c r="H76" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I76" s="43">
-        <x:v>12736</x:v>
+        <x:v>11989.2</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2811,23 +2809,23 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C77" s="41">
-        <x:v>1062</x:v>
+        <x:v>1162</x:v>
       </x:c>
       <x:c r="D77" s="40"/>
       <x:c r="E77" s="42">
-        <x:v>32576</x:v>
+        <x:v>34494</x:v>
       </x:c>
       <x:c r="F77" s="42">
-        <x:v>32575</x:v>
+        <x:v>34494</x:v>
       </x:c>
       <x:c r="G77" s="43">
-        <x:v>18320</x:v>
+        <x:v>3153</x:v>
       </x:c>
       <x:c r="H77" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I77" s="43">
-        <x:v>18320</x:v>
+        <x:v>3153</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:11" ht="10.2" customHeight="1" outlineLevel="1">
@@ -2889,23 +2887,23 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="C81" s="41">
-        <x:v>1205</x:v>
+        <x:v>1166</x:v>
       </x:c>
       <x:c r="D81" s="40"/>
       <x:c r="E81" s="42">
-        <x:v>34628</x:v>
+        <x:v>34516</x:v>
       </x:c>
       <x:c r="F81" s="42">
-        <x:v>34628</x:v>
+        <x:v>34516</x:v>
       </x:c>
       <x:c r="G81" s="43">
-        <x:v>4029.55</x:v>
+        <x:v>28862</x:v>
       </x:c>
       <x:c r="H81" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I81" s="43">
-        <x:v>4029.55</x:v>
+        <x:v>28862</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -2913,23 +2911,23 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="C82" s="41">
-        <x:v>1166</x:v>
+        <x:v>1205</x:v>
       </x:c>
       <x:c r="D82" s="40"/>
       <x:c r="E82" s="42">
-        <x:v>34516</x:v>
+        <x:v>34628</x:v>
       </x:c>
       <x:c r="F82" s="42">
-        <x:v>34516</x:v>
+        <x:v>34628</x:v>
       </x:c>
       <x:c r="G82" s="43">
-        <x:v>28862</x:v>
+        <x:v>4029.55</x:v>
       </x:c>
       <x:c r="H82" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I82" s="43">
-        <x:v>28862</x:v>
+        <x:v>4029.55</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:11" ht="10.2" customHeight="1" outlineLevel="1">
@@ -3217,25 +3215,25 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="C98" s="41">
-        <x:v>1295</x:v>
+        <x:v>1095</x:v>
       </x:c>
       <x:c r="D98" s="40" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="E98" s="42">
-        <x:v>34705</x:v>
+        <x:v>32665</x:v>
       </x:c>
       <x:c r="F98" s="42">
-        <x:v>34705</x:v>
+        <x:v>32664</x:v>
       </x:c>
       <x:c r="G98" s="43">
-        <x:v>17917</x:v>
+        <x:v>7531.75</x:v>
       </x:c>
       <x:c r="H98" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I98" s="43">
-        <x:v>17917</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="99" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -3243,23 +3241,23 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="C99" s="41">
-        <x:v>1095</x:v>
+        <x:v>1295</x:v>
       </x:c>
       <x:c r="D99" s="40"/>
       <x:c r="E99" s="42">
-        <x:v>32665</x:v>
+        <x:v>34705</x:v>
       </x:c>
       <x:c r="F99" s="42">
-        <x:v>32664</x:v>
+        <x:v>34705</x:v>
       </x:c>
       <x:c r="G99" s="43">
-        <x:v>7531.75</x:v>
+        <x:v>17917</x:v>
       </x:c>
       <x:c r="H99" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I99" s="43">
-        <x:v>0</x:v>
+        <x:v>17917</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="1:11" ht="10.2" customHeight="1" outlineLevel="1">
@@ -3479,23 +3477,23 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="C111" s="41">
-        <x:v>1298</x:v>
+        <x:v>1198</x:v>
       </x:c>
       <x:c r="D111" s="40"/>
       <x:c r="E111" s="42">
-        <x:v>34708</x:v>
+        <x:v>34591</x:v>
       </x:c>
       <x:c r="F111" s="42">
-        <x:v>34708</x:v>
+        <x:v>34591</x:v>
       </x:c>
       <x:c r="G111" s="43">
-        <x:v>9897</x:v>
+        <x:v>72089.9</x:v>
       </x:c>
       <x:c r="H111" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I111" s="43">
-        <x:v>9897</x:v>
+        <x:v>72089.9</x:v>
       </x:c>
     </x:row>
     <x:row r="112" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -3503,23 +3501,23 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="C112" s="41">
-        <x:v>1198</x:v>
+        <x:v>1298</x:v>
       </x:c>
       <x:c r="D112" s="40"/>
       <x:c r="E112" s="42">
-        <x:v>34591</x:v>
+        <x:v>34708</x:v>
       </x:c>
       <x:c r="F112" s="42">
-        <x:v>34591</x:v>
+        <x:v>34708</x:v>
       </x:c>
       <x:c r="G112" s="43">
-        <x:v>72089.9</x:v>
+        <x:v>9897</x:v>
       </x:c>
       <x:c r="H112" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I112" s="43">
-        <x:v>72089.9</x:v>
+        <x:v>9897</x:v>
       </x:c>
     </x:row>
     <x:row r="113" spans="1:11" ht="10.2" customHeight="1" outlineLevel="1">
@@ -3727,25 +3725,25 @@
         <x:v>57</x:v>
       </x:c>
       <x:c r="C124" s="41">
-        <x:v>1209</x:v>
+        <x:v>1009</x:v>
       </x:c>
       <x:c r="D124" s="40" t="s">
         <x:v>59</x:v>
       </x:c>
       <x:c r="E124" s="42">
-        <x:v>34650</x:v>
+        <x:v>32275</x:v>
       </x:c>
       <x:c r="F124" s="42">
-        <x:v>34650</x:v>
+        <x:v>32274</x:v>
       </x:c>
       <x:c r="G124" s="43">
-        <x:v>20711.9</x:v>
+        <x:v>5587</x:v>
       </x:c>
       <x:c r="H124" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I124" s="43">
-        <x:v>20711.9</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="125" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -3777,23 +3775,23 @@
         <x:v>57</x:v>
       </x:c>
       <x:c r="C126" s="41">
-        <x:v>1009</x:v>
+        <x:v>1209</x:v>
       </x:c>
       <x:c r="D126" s="40"/>
       <x:c r="E126" s="42">
-        <x:v>32275</x:v>
+        <x:v>34650</x:v>
       </x:c>
       <x:c r="F126" s="42">
-        <x:v>32274</x:v>
+        <x:v>34650</x:v>
       </x:c>
       <x:c r="G126" s="43">
-        <x:v>5587</x:v>
+        <x:v>20711.9</x:v>
       </x:c>
       <x:c r="H126" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I126" s="43">
-        <x:v>0</x:v>
+        <x:v>20711.9</x:v>
       </x:c>
     </x:row>
     <x:row r="127" spans="1:11" ht="10.2" customHeight="1" outlineLevel="2">
@@ -3881,23 +3879,23 @@
         <x:v>57</x:v>
       </x:c>
       <x:c r="C131" s="41">
-        <x:v>1197</x:v>
+        <x:v>1156</x:v>
       </x:c>
       <x:c r="D131" s="40"/>
       <x:c r="E131" s="42">
-        <x:v>34589</x:v>
+        <x:v>34463</x:v>
       </x:c>
       <x:c r="F131" s="42">
-        <x:v>34589</x:v>
+        <x:v>34463</x:v>
       </x:c>
       <x:c r="G131" s="43">
-        <x:v>6731</x:v>
+        <x:v>12367</x:v>
       </x:c>
       <x:c r="H131" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I131" s="43">
-        <x:v>6731</x:v>
+        <x:v>12367</x:v>
       </x:c>
     </x:row>
     <x:row r="132" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -3905,23 +3903,23 @@
         <x:v>57</x:v>
       </x:c>
       <x:c r="C132" s="41">
-        <x:v>1156</x:v>
+        <x:v>1197</x:v>
       </x:c>
       <x:c r="D132" s="40"/>
       <x:c r="E132" s="42">
-        <x:v>34463</x:v>
+        <x:v>34589</x:v>
       </x:c>
       <x:c r="F132" s="42">
-        <x:v>34463</x:v>
+        <x:v>34589</x:v>
       </x:c>
       <x:c r="G132" s="43">
-        <x:v>12367</x:v>
+        <x:v>6731</x:v>
       </x:c>
       <x:c r="H132" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I132" s="43">
-        <x:v>12367</x:v>
+        <x:v>6731</x:v>
       </x:c>
     </x:row>
     <x:row r="133" spans="1:11" ht="10.2" customHeight="1" outlineLevel="2">
@@ -4279,25 +4277,25 @@
         <x:v>67</x:v>
       </x:c>
       <x:c r="C152" s="41">
-        <x:v>1103</x:v>
+        <x:v>1063</x:v>
       </x:c>
       <x:c r="D152" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E152" s="42">
-        <x:v>33798</x:v>
+        <x:v>32581</x:v>
       </x:c>
       <x:c r="F152" s="42">
-        <x:v>33798</x:v>
+        <x:v>32580</x:v>
       </x:c>
       <x:c r="G152" s="43">
-        <x:v>39797.7</x:v>
+        <x:v>61869.3</x:v>
       </x:c>
       <x:c r="H152" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I152" s="43">
-        <x:v>39797.7</x:v>
+        <x:v>61869.3</x:v>
       </x:c>
     </x:row>
     <x:row r="153" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -4305,23 +4303,23 @@
         <x:v>67</x:v>
       </x:c>
       <x:c r="C153" s="41">
-        <x:v>1063</x:v>
+        <x:v>1103</x:v>
       </x:c>
       <x:c r="D153" s="40"/>
       <x:c r="E153" s="42">
-        <x:v>32581</x:v>
+        <x:v>33798</x:v>
       </x:c>
       <x:c r="F153" s="42">
-        <x:v>32580</x:v>
+        <x:v>33798</x:v>
       </x:c>
       <x:c r="G153" s="43">
-        <x:v>61869.3</x:v>
+        <x:v>39797.7</x:v>
       </x:c>
       <x:c r="H153" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I153" s="43">
-        <x:v>61869.3</x:v>
+        <x:v>39797.7</x:v>
       </x:c>
     </x:row>
     <x:row r="154" spans="1:11" ht="10.2" customHeight="1" outlineLevel="1">
@@ -4581,23 +4579,23 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="C167" s="41">
-        <x:v>1315</x:v>
+        <x:v>1215</x:v>
       </x:c>
       <x:c r="D167" s="40"/>
       <x:c r="E167" s="42">
-        <x:v>34725</x:v>
+        <x:v>34654</x:v>
       </x:c>
       <x:c r="F167" s="42">
-        <x:v>34725</x:v>
+        <x:v>34654</x:v>
       </x:c>
       <x:c r="G167" s="43">
-        <x:v>5037.1</x:v>
+        <x:v>8305.95</x:v>
       </x:c>
       <x:c r="H167" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I167" s="43">
-        <x:v>5037.1</x:v>
+        <x:v>8305.95</x:v>
       </x:c>
     </x:row>
     <x:row r="168" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -4605,23 +4603,23 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="C168" s="41">
-        <x:v>1215</x:v>
+        <x:v>1315</x:v>
       </x:c>
       <x:c r="D168" s="40"/>
       <x:c r="E168" s="42">
-        <x:v>34654</x:v>
+        <x:v>34725</x:v>
       </x:c>
       <x:c r="F168" s="42">
-        <x:v>34654</x:v>
+        <x:v>34725</x:v>
       </x:c>
       <x:c r="G168" s="43">
-        <x:v>8305.95</x:v>
+        <x:v>5037.1</x:v>
       </x:c>
       <x:c r="H168" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I168" s="43">
-        <x:v>8305.95</x:v>
+        <x:v>5037.1</x:v>
       </x:c>
     </x:row>
     <x:row r="169" spans="1:11" ht="10.2" customHeight="1" outlineLevel="2">
@@ -4643,25 +4641,25 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="C170" s="41">
-        <x:v>1128</x:v>
+        <x:v>1028</x:v>
       </x:c>
       <x:c r="D170" s="40" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="E170" s="42">
-        <x:v>34250</x:v>
+        <x:v>32332</x:v>
       </x:c>
       <x:c r="F170" s="42">
-        <x:v>34250</x:v>
+        <x:v>32331</x:v>
       </x:c>
       <x:c r="G170" s="43">
-        <x:v>8294</x:v>
+        <x:v>343.8</x:v>
       </x:c>
       <x:c r="H170" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I170" s="43">
-        <x:v>8294</x:v>
+        <x:v>343.8</x:v>
       </x:c>
     </x:row>
     <x:row r="171" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -4669,23 +4667,23 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="C171" s="41">
-        <x:v>1028</x:v>
+        <x:v>1128</x:v>
       </x:c>
       <x:c r="D171" s="40"/>
       <x:c r="E171" s="42">
-        <x:v>32332</x:v>
+        <x:v>34250</x:v>
       </x:c>
       <x:c r="F171" s="42">
-        <x:v>32331</x:v>
+        <x:v>34250</x:v>
       </x:c>
       <x:c r="G171" s="43">
-        <x:v>343.8</x:v>
+        <x:v>8294</x:v>
       </x:c>
       <x:c r="H171" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I171" s="43">
-        <x:v>343.8</x:v>
+        <x:v>8294</x:v>
       </x:c>
     </x:row>
     <x:row r="172" spans="1:11" ht="10.2" customHeight="1" outlineLevel="1">
@@ -4721,25 +4719,25 @@
         <x:v>73</x:v>
       </x:c>
       <x:c r="C174" s="41">
-        <x:v>1141</x:v>
+        <x:v>1041</x:v>
       </x:c>
       <x:c r="D174" s="40" t="s">
         <x:v>31</x:v>
       </x:c>
       <x:c r="E174" s="42">
-        <x:v>34320</x:v>
+        <x:v>32403</x:v>
       </x:c>
       <x:c r="F174" s="42">
-        <x:v>34320</x:v>
+        <x:v>32402</x:v>
       </x:c>
       <x:c r="G174" s="43">
-        <x:v>1846</x:v>
+        <x:v>7807</x:v>
       </x:c>
       <x:c r="H174" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I174" s="43">
-        <x:v>1846</x:v>
+        <x:v>7807</x:v>
       </x:c>
     </x:row>
     <x:row r="175" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -4747,23 +4745,23 @@
         <x:v>73</x:v>
       </x:c>
       <x:c r="C175" s="41">
-        <x:v>1041</x:v>
+        <x:v>1141</x:v>
       </x:c>
       <x:c r="D175" s="40"/>
       <x:c r="E175" s="42">
-        <x:v>32403</x:v>
+        <x:v>34320</x:v>
       </x:c>
       <x:c r="F175" s="42">
-        <x:v>32402</x:v>
+        <x:v>34320</x:v>
       </x:c>
       <x:c r="G175" s="43">
-        <x:v>7807</x:v>
+        <x:v>1846</x:v>
       </x:c>
       <x:c r="H175" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I175" s="43">
-        <x:v>7807</x:v>
+        <x:v>1846</x:v>
       </x:c>
     </x:row>
     <x:row r="176" spans="1:11" ht="10.2" customHeight="1" outlineLevel="1">
@@ -4863,25 +4861,25 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="C181" s="41">
-        <x:v>1269</x:v>
+        <x:v>1169</x:v>
       </x:c>
       <x:c r="D181" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E181" s="42">
-        <x:v>34684</x:v>
+        <x:v>34521</x:v>
       </x:c>
       <x:c r="F181" s="42">
-        <x:v>34684</x:v>
+        <x:v>34521</x:v>
       </x:c>
       <x:c r="G181" s="43">
-        <x:v>1400</x:v>
+        <x:v>9471.95</x:v>
       </x:c>
       <x:c r="H181" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I181" s="43">
-        <x:v>1400</x:v>
+        <x:v>9471.95</x:v>
       </x:c>
     </x:row>
     <x:row r="182" spans="1:11" ht="10.2" customHeight="1" outlineLevel="3">
@@ -4889,23 +4887,23 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="C182" s="41">
-        <x:v>1169</x:v>
+        <x:v>1269</x:v>
       </x:c>
       <x:c r="D182" s="40"/>
       <x:c r="E182" s="42">
-        <x:v>34521</x:v>
+        <x:v>34684</x:v>
       </x:c>
       <x:c r="F182" s="42">
-        <x:v>34521</x:v>
+        <x:v>34684</x:v>
       </x:c>
       <x:c r="G182" s="43">
-        <x:v>9471.95</x:v>
+        <x:v>1400</x:v>
       </x:c>
       <x:c r="H182" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I182" s="43">
-        <x:v>9471.95</x:v>
+        <x:v>1400</x:v>
       </x:c>
     </x:row>
     <x:row r="183" spans="1:11" ht="10.2" customHeight="1" outlineLevel="2">
@@ -5515,25 +5513,25 @@
         <x:v>85</x:v>
       </x:c>
       <x:c r="C214" s="41">
-        <x:v>1170</x:v>
+        <x:v>1077</x:v>
       </x:c>
       <x:c r="D214" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E214" s="42">
-        <x:v>34523</x:v>
+        <x:v>32629</x:v>
       </x:c>
       <x:c r="F214" s="42">
-        <x:v>34523</x:v>
+        <x:v>32627</x:v>
       </x:c>
       <x:c r="G214" s="43">
-        <x:v>5654.8</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="H214" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I214" s="43">
-        <x:v>5654.8</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="215" spans="1:11" outlineLevel="3">
@@ -5541,23 +5539,23 @@
         <x:v>85</x:v>
       </x:c>
       <x:c r="C215" s="41">
-        <x:v>1077</x:v>
+        <x:v>1170</x:v>
       </x:c>
       <x:c r="D215" s="40"/>
       <x:c r="E215" s="42">
-        <x:v>32629</x:v>
+        <x:v>34523</x:v>
       </x:c>
       <x:c r="F215" s="42">
-        <x:v>32627</x:v>
+        <x:v>34523</x:v>
       </x:c>
       <x:c r="G215" s="43">
-        <x:v>156</x:v>
+        <x:v>5654.8</x:v>
       </x:c>
       <x:c r="H215" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I215" s="43">
-        <x:v>156</x:v>
+        <x:v>5654.8</x:v>
       </x:c>
     </x:row>
     <x:row r="216" spans="1:11" outlineLevel="1">
@@ -5657,25 +5655,25 @@
         <x:v>87</x:v>
       </x:c>
       <x:c r="C221" s="41">
-        <x:v>1149</x:v>
+        <x:v>1049</x:v>
       </x:c>
       <x:c r="D221" s="40" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="E221" s="42">
-        <x:v>34407</x:v>
+        <x:v>32491</x:v>
       </x:c>
       <x:c r="F221" s="42">
-        <x:v>34407</x:v>
+        <x:v>32490</x:v>
       </x:c>
       <x:c r="G221" s="43">
-        <x:v>12900.75</x:v>
+        <x:v>1809.85</x:v>
       </x:c>
       <x:c r="H221" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I221" s="43">
-        <x:v>12900.75</x:v>
+        <x:v>1809.85</x:v>
       </x:c>
     </x:row>
     <x:row r="222" spans="1:11" outlineLevel="3">
@@ -5683,23 +5681,23 @@
         <x:v>87</x:v>
       </x:c>
       <x:c r="C222" s="41">
-        <x:v>1049</x:v>
+        <x:v>1149</x:v>
       </x:c>
       <x:c r="D222" s="40"/>
       <x:c r="E222" s="42">
-        <x:v>32491</x:v>
+        <x:v>34407</x:v>
       </x:c>
       <x:c r="F222" s="42">
-        <x:v>32490</x:v>
+        <x:v>34407</x:v>
       </x:c>
       <x:c r="G222" s="43">
-        <x:v>1809.85</x:v>
+        <x:v>12900.75</x:v>
       </x:c>
       <x:c r="H222" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I222" s="43">
-        <x:v>1809.85</x:v>
+        <x:v>12900.75</x:v>
       </x:c>
     </x:row>
     <x:row r="223" spans="1:11" outlineLevel="1">
@@ -5829,25 +5827,25 @@
         <x:v>91</x:v>
       </x:c>
       <x:c r="C230" s="41">
-        <x:v>1144</x:v>
+        <x:v>1044</x:v>
       </x:c>
       <x:c r="D230" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E230" s="42">
-        <x:v>34343</x:v>
+        <x:v>32425</x:v>
       </x:c>
       <x:c r="F230" s="42">
-        <x:v>34343</x:v>
+        <x:v>32424</x:v>
       </x:c>
       <x:c r="G230" s="43">
-        <x:v>10054</x:v>
+        <x:v>64050</x:v>
       </x:c>
       <x:c r="H230" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I230" s="43">
-        <x:v>10054</x:v>
+        <x:v>64050</x:v>
       </x:c>
     </x:row>
     <x:row r="231" spans="1:11" outlineLevel="3">
@@ -5855,23 +5853,23 @@
         <x:v>91</x:v>
       </x:c>
       <x:c r="C231" s="41">
-        <x:v>1044</x:v>
+        <x:v>1144</x:v>
       </x:c>
       <x:c r="D231" s="40"/>
       <x:c r="E231" s="42">
-        <x:v>32425</x:v>
+        <x:v>34343</x:v>
       </x:c>
       <x:c r="F231" s="42">
-        <x:v>32424</x:v>
+        <x:v>34343</x:v>
       </x:c>
       <x:c r="G231" s="43">
-        <x:v>64050</x:v>
+        <x:v>10054</x:v>
       </x:c>
       <x:c r="H231" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I231" s="43">
-        <x:v>64050</x:v>
+        <x:v>10054</x:v>
       </x:c>
     </x:row>
     <x:row r="232" spans="1:11" outlineLevel="1">
@@ -6463,25 +6461,25 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="C263" s="41">
-        <x:v>1132</x:v>
+        <x:v>1021</x:v>
       </x:c>
       <x:c r="D263" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E263" s="42">
-        <x:v>34274</x:v>
+        <x:v>32319</x:v>
       </x:c>
       <x:c r="F263" s="42">
-        <x:v>34274</x:v>
+        <x:v>32318</x:v>
       </x:c>
       <x:c r="G263" s="43">
-        <x:v>906</x:v>
+        <x:v>3719</x:v>
       </x:c>
       <x:c r="H263" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I263" s="43">
-        <x:v>906</x:v>
+        <x:v>3719</x:v>
       </x:c>
     </x:row>
     <x:row r="264" spans="1:11" outlineLevel="3">
@@ -6489,23 +6487,23 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="C264" s="41">
-        <x:v>1221</x:v>
+        <x:v>1022</x:v>
       </x:c>
       <x:c r="D264" s="40"/>
       <x:c r="E264" s="42">
-        <x:v>34661</x:v>
+        <x:v>32325</x:v>
       </x:c>
       <x:c r="F264" s="42">
-        <x:v>34661</x:v>
+        <x:v>32324</x:v>
       </x:c>
       <x:c r="G264" s="43">
-        <x:v>2099</x:v>
+        <x:v>10064.65</x:v>
       </x:c>
       <x:c r="H264" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I264" s="43">
-        <x:v>2099</x:v>
+        <x:v>10064.65</x:v>
       </x:c>
     </x:row>
     <x:row r="265" spans="1:11" outlineLevel="3">
@@ -6513,23 +6511,23 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="C265" s="41">
-        <x:v>1136</x:v>
+        <x:v>1032</x:v>
       </x:c>
       <x:c r="D265" s="40"/>
       <x:c r="E265" s="42">
-        <x:v>34300</x:v>
+        <x:v>32356</x:v>
       </x:c>
       <x:c r="F265" s="42">
-        <x:v>34300</x:v>
+        <x:v>32352</x:v>
       </x:c>
       <x:c r="G265" s="43">
-        <x:v>2971</x:v>
+        <x:v>775</x:v>
       </x:c>
       <x:c r="H265" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I265" s="43">
-        <x:v>2971</x:v>
+        <x:v>775</x:v>
       </x:c>
     </x:row>
     <x:row r="266" spans="1:11" outlineLevel="3">
@@ -6537,23 +6535,23 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="C266" s="41">
-        <x:v>1021</x:v>
+        <x:v>1121</x:v>
       </x:c>
       <x:c r="D266" s="40"/>
       <x:c r="E266" s="42">
-        <x:v>32319</x:v>
+        <x:v>34122</x:v>
       </x:c>
       <x:c r="F266" s="42">
-        <x:v>32318</x:v>
+        <x:v>34122</x:v>
       </x:c>
       <x:c r="G266" s="43">
-        <x:v>3719</x:v>
+        <x:v>820</x:v>
       </x:c>
       <x:c r="H266" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I266" s="43">
-        <x:v>3719</x:v>
+        <x:v>820</x:v>
       </x:c>
     </x:row>
     <x:row r="267" spans="1:11" outlineLevel="3">
@@ -6561,23 +6559,23 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="C267" s="41">
-        <x:v>1032</x:v>
+        <x:v>1122</x:v>
       </x:c>
       <x:c r="D267" s="40"/>
       <x:c r="E267" s="42">
-        <x:v>32356</x:v>
+        <x:v>34173</x:v>
       </x:c>
       <x:c r="F267" s="42">
-        <x:v>32352</x:v>
+        <x:v>34173</x:v>
       </x:c>
       <x:c r="G267" s="43">
-        <x:v>775</x:v>
+        <x:v>44854</x:v>
       </x:c>
       <x:c r="H267" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I267" s="43">
-        <x:v>775</x:v>
+        <x:v>44854</x:v>
       </x:c>
     </x:row>
     <x:row r="268" spans="1:11" outlineLevel="3">
@@ -6585,23 +6583,23 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="C268" s="41">
-        <x:v>1122</x:v>
+        <x:v>1132</x:v>
       </x:c>
       <x:c r="D268" s="40"/>
       <x:c r="E268" s="42">
-        <x:v>34173</x:v>
+        <x:v>34274</x:v>
       </x:c>
       <x:c r="F268" s="42">
-        <x:v>34173</x:v>
+        <x:v>34274</x:v>
       </x:c>
       <x:c r="G268" s="43">
-        <x:v>44854</x:v>
+        <x:v>906</x:v>
       </x:c>
       <x:c r="H268" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I268" s="43">
-        <x:v>44854</x:v>
+        <x:v>906</x:v>
       </x:c>
     </x:row>
     <x:row r="269" spans="1:11" outlineLevel="3">
@@ -6609,23 +6607,23 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="C269" s="41">
-        <x:v>1121</x:v>
+        <x:v>1136</x:v>
       </x:c>
       <x:c r="D269" s="40"/>
       <x:c r="E269" s="42">
-        <x:v>34122</x:v>
+        <x:v>34300</x:v>
       </x:c>
       <x:c r="F269" s="42">
-        <x:v>34122</x:v>
+        <x:v>34300</x:v>
       </x:c>
       <x:c r="G269" s="43">
-        <x:v>820</x:v>
+        <x:v>2971</x:v>
       </x:c>
       <x:c r="H269" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I269" s="43">
-        <x:v>820</x:v>
+        <x:v>2971</x:v>
       </x:c>
     </x:row>
     <x:row r="270" spans="1:11" outlineLevel="3">
@@ -6633,23 +6631,23 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="C270" s="41">
-        <x:v>1022</x:v>
+        <x:v>1221</x:v>
       </x:c>
       <x:c r="D270" s="40"/>
       <x:c r="E270" s="42">
-        <x:v>32325</x:v>
+        <x:v>34661</x:v>
       </x:c>
       <x:c r="F270" s="42">
-        <x:v>32324</x:v>
+        <x:v>34661</x:v>
       </x:c>
       <x:c r="G270" s="43">
-        <x:v>10064.65</x:v>
+        <x:v>2099</x:v>
       </x:c>
       <x:c r="H270" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I270" s="43">
-        <x:v>10064.65</x:v>
+        <x:v>2099</x:v>
       </x:c>
     </x:row>
     <x:row r="271" spans="1:11" outlineLevel="1">
@@ -6685,25 +6683,25 @@
         <x:v>107</x:v>
       </x:c>
       <x:c r="C273" s="41">
-        <x:v>1101</x:v>
+        <x:v>1051</x:v>
       </x:c>
       <x:c r="D273" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E273" s="42">
-        <x:v>32693</x:v>
+        <x:v>32513</x:v>
       </x:c>
       <x:c r="F273" s="42">
-        <x:v>32693</x:v>
+        <x:v>32512</x:v>
       </x:c>
       <x:c r="G273" s="43">
-        <x:v>11629.85</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="H273" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I273" s="43">
-        <x:v>0</x:v>
+        <x:v>325</x:v>
       </x:c>
     </x:row>
     <x:row r="274" spans="1:11" outlineLevel="3">
@@ -6711,23 +6709,23 @@
         <x:v>107</x:v>
       </x:c>
       <x:c r="C274" s="41">
-        <x:v>1051</x:v>
+        <x:v>1101</x:v>
       </x:c>
       <x:c r="D274" s="40"/>
       <x:c r="E274" s="42">
-        <x:v>32513</x:v>
+        <x:v>32693</x:v>
       </x:c>
       <x:c r="F274" s="42">
-        <x:v>32512</x:v>
+        <x:v>32693</x:v>
       </x:c>
       <x:c r="G274" s="43">
-        <x:v>325</x:v>
+        <x:v>11629.85</x:v>
       </x:c>
       <x:c r="H274" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I274" s="43">
-        <x:v>325</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="275" spans="1:11" outlineLevel="1">
@@ -6763,25 +6761,25 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="C277" s="41">
-        <x:v>1052</x:v>
+        <x:v>1003</x:v>
       </x:c>
       <x:c r="D277" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E277" s="42">
-        <x:v>32515</x:v>
+        <x:v>32266</x:v>
       </x:c>
       <x:c r="F277" s="42">
-        <x:v>32514</x:v>
+        <x:v>32245</x:v>
       </x:c>
       <x:c r="G277" s="43">
-        <x:v>16788</x:v>
+        <x:v>1250</x:v>
       </x:c>
       <x:c r="H277" s="43">
-        <x:v>0</x:v>
+        <x:v>4.5</x:v>
       </x:c>
       <x:c r="I277" s="43">
-        <x:v>16788</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="278" spans="1:11" outlineLevel="3">
@@ -6789,23 +6787,23 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="C278" s="41">
-        <x:v>1155</x:v>
+        <x:v>1052</x:v>
       </x:c>
       <x:c r="D278" s="40"/>
       <x:c r="E278" s="42">
-        <x:v>34459</x:v>
+        <x:v>32515</x:v>
       </x:c>
       <x:c r="F278" s="42">
-        <x:v>34459</x:v>
+        <x:v>32514</x:v>
       </x:c>
       <x:c r="G278" s="43">
-        <x:v>13935.95</x:v>
+        <x:v>16788</x:v>
       </x:c>
       <x:c r="H278" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I278" s="43">
-        <x:v>13935.95</x:v>
+        <x:v>16788</x:v>
       </x:c>
     </x:row>
     <x:row r="279" spans="1:11" outlineLevel="3">
@@ -6813,23 +6811,23 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="C279" s="41">
-        <x:v>1152</x:v>
+        <x:v>1055</x:v>
       </x:c>
       <x:c r="D279" s="40"/>
       <x:c r="E279" s="42">
-        <x:v>34431</x:v>
+        <x:v>32544</x:v>
       </x:c>
       <x:c r="F279" s="42">
-        <x:v>34431</x:v>
+        <x:v>32543</x:v>
       </x:c>
       <x:c r="G279" s="43">
-        <x:v>97698.6</x:v>
+        <x:v>23406</x:v>
       </x:c>
       <x:c r="H279" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I279" s="43">
-        <x:v>97698.6</x:v>
+        <x:v>23406</x:v>
       </x:c>
     </x:row>
     <x:row r="280" spans="1:11" outlineLevel="3">
@@ -6837,23 +6835,23 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="C280" s="41">
-        <x:v>1163</x:v>
+        <x:v>1087</x:v>
       </x:c>
       <x:c r="D280" s="40"/>
       <x:c r="E280" s="42">
-        <x:v>34499</x:v>
+        <x:v>32649</x:v>
       </x:c>
       <x:c r="F280" s="42">
-        <x:v>34499</x:v>
+        <x:v>32648</x:v>
       </x:c>
       <x:c r="G280" s="43">
-        <x:v>342</x:v>
+        <x:v>14045</x:v>
       </x:c>
       <x:c r="H280" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I280" s="43">
-        <x:v>342</x:v>
+        <x:v>14045</x:v>
       </x:c>
     </x:row>
     <x:row r="281" spans="1:11" outlineLevel="3">
@@ -6861,23 +6859,23 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="C281" s="41">
-        <x:v>1087</x:v>
+        <x:v>1152</x:v>
       </x:c>
       <x:c r="D281" s="40"/>
       <x:c r="E281" s="42">
-        <x:v>32649</x:v>
+        <x:v>34431</x:v>
       </x:c>
       <x:c r="F281" s="42">
-        <x:v>32648</x:v>
+        <x:v>34431</x:v>
       </x:c>
       <x:c r="G281" s="43">
-        <x:v>14045</x:v>
+        <x:v>97698.6</x:v>
       </x:c>
       <x:c r="H281" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I281" s="43">
-        <x:v>14045</x:v>
+        <x:v>97698.6</x:v>
       </x:c>
     </x:row>
     <x:row r="282" spans="1:11" outlineLevel="3">
@@ -6885,23 +6883,23 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="C282" s="41">
-        <x:v>1055</x:v>
+        <x:v>1155</x:v>
       </x:c>
       <x:c r="D282" s="40"/>
       <x:c r="E282" s="42">
-        <x:v>32544</x:v>
+        <x:v>34459</x:v>
       </x:c>
       <x:c r="F282" s="42">
-        <x:v>32543</x:v>
+        <x:v>34459</x:v>
       </x:c>
       <x:c r="G282" s="43">
-        <x:v>23406</x:v>
+        <x:v>13935.95</x:v>
       </x:c>
       <x:c r="H282" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I282" s="43">
-        <x:v>23406</x:v>
+        <x:v>13935.95</x:v>
       </x:c>
     </x:row>
     <x:row r="283" spans="1:11" outlineLevel="3">
@@ -6909,23 +6907,23 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="C283" s="41">
-        <x:v>1003</x:v>
+        <x:v>1163</x:v>
       </x:c>
       <x:c r="D283" s="40"/>
       <x:c r="E283" s="42">
-        <x:v>32266</x:v>
+        <x:v>34499</x:v>
       </x:c>
       <x:c r="F283" s="42">
-        <x:v>32245</x:v>
+        <x:v>34499</x:v>
       </x:c>
       <x:c r="G283" s="43">
-        <x:v>1250</x:v>
+        <x:v>342</x:v>
       </x:c>
       <x:c r="H283" s="43">
-        <x:v>4.5</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="I283" s="43">
-        <x:v>0</x:v>
+        <x:v>342</x:v>
       </x:c>
     </x:row>
     <x:row r="284" spans="1:11" outlineLevel="3">
@@ -6971,25 +6969,25 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="C286" s="41">
-        <x:v>1275</x:v>
+        <x:v>1075</x:v>
       </x:c>
       <x:c r="D286" s="40" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="E286" s="42">
-        <x:v>34690</x:v>
+        <x:v>32620</x:v>
       </x:c>
       <x:c r="F286" s="42">
-        <x:v>34690</x:v>
+        <x:v>32619</x:v>
       </x:c>
       <x:c r="G286" s="43">
-        <x:v>16939.5</x:v>
+        <x:v>8560</x:v>
       </x:c>
       <x:c r="H286" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I286" s="43">
-        <x:v>16939.5</x:v>
+        <x:v>8560</x:v>
       </x:c>
     </x:row>
     <x:row r="287" spans="1:11" outlineLevel="3">
@@ -6997,23 +6995,23 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="C287" s="41">
-        <x:v>1075</x:v>
+        <x:v>1275</x:v>
       </x:c>
       <x:c r="D287" s="40"/>
       <x:c r="E287" s="42">
-        <x:v>32620</x:v>
+        <x:v>34690</x:v>
       </x:c>
       <x:c r="F287" s="42">
-        <x:v>32619</x:v>
+        <x:v>34690</x:v>
       </x:c>
       <x:c r="G287" s="43">
-        <x:v>8560</x:v>
+        <x:v>16939.5</x:v>
       </x:c>
       <x:c r="H287" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I287" s="43">
-        <x:v>8560</x:v>
+        <x:v>16939.5</x:v>
       </x:c>
     </x:row>
     <x:row r="288" spans="1:11" outlineLevel="2">
@@ -7089,25 +7087,25 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="C292" s="41">
-        <x:v>1171</x:v>
+        <x:v>1071</x:v>
       </x:c>
       <x:c r="D292" s="40" t="s">
         <x:v>37</x:v>
       </x:c>
       <x:c r="E292" s="42">
-        <x:v>34525</x:v>
+        <x:v>32608</x:v>
       </x:c>
       <x:c r="F292" s="42">
-        <x:v>34525</x:v>
+        <x:v>32607</x:v>
       </x:c>
       <x:c r="G292" s="43">
-        <x:v>2356.9</x:v>
+        <x:v>103041</x:v>
       </x:c>
       <x:c r="H292" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I292" s="43">
-        <x:v>2356.9</x:v>
+        <x:v>103041</x:v>
       </x:c>
     </x:row>
     <x:row r="293" spans="1:11" outlineLevel="3">
@@ -7115,23 +7113,23 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="C293" s="41">
-        <x:v>1271</x:v>
+        <x:v>1171</x:v>
       </x:c>
       <x:c r="D293" s="40"/>
       <x:c r="E293" s="42">
-        <x:v>34688</x:v>
+        <x:v>34525</x:v>
       </x:c>
       <x:c r="F293" s="42">
-        <x:v>34688</x:v>
+        <x:v>34525</x:v>
       </x:c>
       <x:c r="G293" s="43">
-        <x:v>304</x:v>
+        <x:v>2356.9</x:v>
       </x:c>
       <x:c r="H293" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I293" s="43">
-        <x:v>304</x:v>
+        <x:v>2356.9</x:v>
       </x:c>
     </x:row>
     <x:row r="294" spans="1:11" outlineLevel="3">
@@ -7139,23 +7137,23 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="C294" s="41">
-        <x:v>1071</x:v>
+        <x:v>1271</x:v>
       </x:c>
       <x:c r="D294" s="40"/>
       <x:c r="E294" s="42">
-        <x:v>32608</x:v>
+        <x:v>34688</x:v>
       </x:c>
       <x:c r="F294" s="42">
-        <x:v>32607</x:v>
+        <x:v>34688</x:v>
       </x:c>
       <x:c r="G294" s="43">
-        <x:v>103041</x:v>
+        <x:v>304</x:v>
       </x:c>
       <x:c r="H294" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I294" s="43">
-        <x:v>103041</x:v>
+        <x:v>304</x:v>
       </x:c>
     </x:row>
     <x:row r="295" spans="1:11" outlineLevel="2">
@@ -7453,25 +7451,25 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="C310" s="41">
-        <x:v>1280</x:v>
+        <x:v>1080</x:v>
       </x:c>
       <x:c r="D310" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E310" s="42">
-        <x:v>34694</x:v>
+        <x:v>32634</x:v>
       </x:c>
       <x:c r="F310" s="42">
-        <x:v>34694</x:v>
+        <x:v>32633</x:v>
       </x:c>
       <x:c r="G310" s="43">
-        <x:v>4317.75</x:v>
+        <x:v>9634</x:v>
       </x:c>
       <x:c r="H310" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I310" s="43">
-        <x:v>4317.75</x:v>
+        <x:v>9634</x:v>
       </x:c>
     </x:row>
     <x:row r="311" spans="1:11" outlineLevel="3">
@@ -7479,23 +7477,23 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="C311" s="41">
-        <x:v>1080</x:v>
+        <x:v>1180</x:v>
       </x:c>
       <x:c r="D311" s="40"/>
       <x:c r="E311" s="42">
-        <x:v>32634</x:v>
+        <x:v>34552</x:v>
       </x:c>
       <x:c r="F311" s="42">
-        <x:v>32633</x:v>
+        <x:v>34552</x:v>
       </x:c>
       <x:c r="G311" s="43">
-        <x:v>9634</x:v>
+        <x:v>3640</x:v>
       </x:c>
       <x:c r="H311" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I311" s="43">
-        <x:v>9634</x:v>
+        <x:v>3640</x:v>
       </x:c>
     </x:row>
     <x:row r="312" spans="1:11" outlineLevel="3">
@@ -7503,23 +7501,23 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="C312" s="41">
-        <x:v>1180</x:v>
+        <x:v>1280</x:v>
       </x:c>
       <x:c r="D312" s="40"/>
       <x:c r="E312" s="42">
-        <x:v>34552</x:v>
+        <x:v>34694</x:v>
       </x:c>
       <x:c r="F312" s="42">
-        <x:v>34552</x:v>
+        <x:v>34694</x:v>
       </x:c>
       <x:c r="G312" s="43">
-        <x:v>3640</x:v>
+        <x:v>4317.75</x:v>
       </x:c>
       <x:c r="H312" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I312" s="43">
-        <x:v>3640</x:v>
+        <x:v>4317.75</x:v>
       </x:c>
     </x:row>
     <x:row r="313" spans="1:11" outlineLevel="2">
@@ -7541,25 +7539,25 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="C314" s="41">
-        <x:v>1105</x:v>
+        <x:v>1005</x:v>
       </x:c>
       <x:c r="D314" s="40" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="E314" s="42">
-        <x:v>33806</x:v>
+        <x:v>32163</x:v>
       </x:c>
       <x:c r="F314" s="42">
-        <x:v>33806</x:v>
+        <x:v>32253</x:v>
       </x:c>
       <x:c r="G314" s="43">
-        <x:v>31219.95</x:v>
+        <x:v>4807</x:v>
       </x:c>
       <x:c r="H314" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I314" s="43">
-        <x:v>31219.95</x:v>
+        <x:v>4807</x:v>
       </x:c>
     </x:row>
     <x:row r="315" spans="1:11" outlineLevel="3">
@@ -7567,23 +7565,23 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="C315" s="41">
-        <x:v>1005</x:v>
+        <x:v>1105</x:v>
       </x:c>
       <x:c r="D315" s="40"/>
       <x:c r="E315" s="42">
-        <x:v>32163</x:v>
+        <x:v>33806</x:v>
       </x:c>
       <x:c r="F315" s="42">
-        <x:v>32253</x:v>
+        <x:v>33806</x:v>
       </x:c>
       <x:c r="G315" s="43">
-        <x:v>4807</x:v>
+        <x:v>31219.95</x:v>
       </x:c>
       <x:c r="H315" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I315" s="43">
-        <x:v>4807</x:v>
+        <x:v>31219.95</x:v>
       </x:c>
     </x:row>
     <x:row r="316" spans="1:11" outlineLevel="3">
@@ -7591,23 +7589,23 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="C316" s="41">
-        <x:v>1305</x:v>
+        <x:v>1266</x:v>
       </x:c>
       <x:c r="D316" s="40"/>
       <x:c r="E316" s="42">
-        <x:v>34719</x:v>
+        <x:v>34683</x:v>
       </x:c>
       <x:c r="F316" s="42">
-        <x:v>34719</x:v>
+        <x:v>34683</x:v>
       </x:c>
       <x:c r="G316" s="43">
-        <x:v>3065</x:v>
+        <x:v>6935</x:v>
       </x:c>
       <x:c r="H316" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I316" s="43">
-        <x:v>3065</x:v>
+        <x:v>6935</x:v>
       </x:c>
     </x:row>
     <x:row r="317" spans="1:11" outlineLevel="3">
@@ -7615,23 +7613,23 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="C317" s="41">
-        <x:v>1266</x:v>
+        <x:v>1305</x:v>
       </x:c>
       <x:c r="D317" s="40"/>
       <x:c r="E317" s="42">
-        <x:v>34683</x:v>
+        <x:v>34719</x:v>
       </x:c>
       <x:c r="F317" s="42">
-        <x:v>34683</x:v>
+        <x:v>34719</x:v>
       </x:c>
       <x:c r="G317" s="43">
-        <x:v>6935</x:v>
+        <x:v>3065</x:v>
       </x:c>
       <x:c r="H317" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I317" s="43">
-        <x:v>6935</x:v>
+        <x:v>3065</x:v>
       </x:c>
     </x:row>
     <x:row r="318" spans="1:11" outlineLevel="1">
@@ -7667,25 +7665,25 @@
         <x:v>117</x:v>
       </x:c>
       <x:c r="C320" s="41">
-        <x:v>1119</x:v>
+        <x:v>1036</x:v>
       </x:c>
       <x:c r="D320" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E320" s="42">
-        <x:v>34104</x:v>
+        <x:v>32381</x:v>
       </x:c>
       <x:c r="F320" s="42">
-        <x:v>34104</x:v>
+        <x:v>32380</x:v>
       </x:c>
       <x:c r="G320" s="43">
-        <x:v>14557.95</x:v>
+        <x:v>4110</x:v>
       </x:c>
       <x:c r="H320" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I320" s="43">
-        <x:v>14557.95</x:v>
+        <x:v>4110</x:v>
       </x:c>
     </x:row>
     <x:row r="321" spans="1:11" outlineLevel="3">
@@ -7693,23 +7691,23 @@
         <x:v>117</x:v>
       </x:c>
       <x:c r="C321" s="41">
-        <x:v>1036</x:v>
+        <x:v>1119</x:v>
       </x:c>
       <x:c r="D321" s="40"/>
       <x:c r="E321" s="42">
-        <x:v>32381</x:v>
+        <x:v>34104</x:v>
       </x:c>
       <x:c r="F321" s="42">
-        <x:v>32380</x:v>
+        <x:v>34104</x:v>
       </x:c>
       <x:c r="G321" s="43">
-        <x:v>4110</x:v>
+        <x:v>14557.95</x:v>
       </x:c>
       <x:c r="H321" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I321" s="43">
-        <x:v>4110</x:v>
+        <x:v>14557.95</x:v>
       </x:c>
     </x:row>
     <x:row r="322" spans="1:11" outlineLevel="2">
@@ -7893,25 +7891,25 @@
         <x:v>123</x:v>
       </x:c>
       <x:c r="C332" s="41">
-        <x:v>1250</x:v>
+        <x:v>1050</x:v>
       </x:c>
       <x:c r="D332" s="40" t="s">
         <x:v>31</x:v>
       </x:c>
       <x:c r="E332" s="42">
-        <x:v>34662</x:v>
+        <x:v>32502</x:v>
       </x:c>
       <x:c r="F332" s="42">
-        <x:v>34662</x:v>
+        <x:v>32501</x:v>
       </x:c>
       <x:c r="G332" s="43">
-        <x:v>45160.1</x:v>
+        <x:v>6287.85</x:v>
       </x:c>
       <x:c r="H332" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I332" s="43">
-        <x:v>45160.1</x:v>
+        <x:v>6287.85</x:v>
       </x:c>
     </x:row>
     <x:row r="333" spans="1:11" outlineLevel="3">
@@ -7919,23 +7917,23 @@
         <x:v>123</x:v>
       </x:c>
       <x:c r="C333" s="41">
-        <x:v>1350</x:v>
+        <x:v>1150</x:v>
       </x:c>
       <x:c r="D333" s="40"/>
       <x:c r="E333" s="42">
-        <x:v>34732</x:v>
+        <x:v>34418</x:v>
       </x:c>
       <x:c r="F333" s="42">
-        <x:v>34732</x:v>
+        <x:v>34418</x:v>
       </x:c>
       <x:c r="G333" s="43">
-        <x:v>8939.6</x:v>
+        <x:v>7671.9</x:v>
       </x:c>
       <x:c r="H333" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I333" s="43">
-        <x:v>8939.6</x:v>
+        <x:v>7671.9</x:v>
       </x:c>
     </x:row>
     <x:row r="334" spans="1:11" outlineLevel="3">
@@ -7943,23 +7941,23 @@
         <x:v>123</x:v>
       </x:c>
       <x:c r="C334" s="41">
-        <x:v>1050</x:v>
+        <x:v>1250</x:v>
       </x:c>
       <x:c r="D334" s="40"/>
       <x:c r="E334" s="42">
-        <x:v>32502</x:v>
+        <x:v>34662</x:v>
       </x:c>
       <x:c r="F334" s="42">
-        <x:v>32501</x:v>
+        <x:v>34662</x:v>
       </x:c>
       <x:c r="G334" s="43">
-        <x:v>6287.85</x:v>
+        <x:v>45160.1</x:v>
       </x:c>
       <x:c r="H334" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I334" s="43">
-        <x:v>6287.85</x:v>
+        <x:v>45160.1</x:v>
       </x:c>
     </x:row>
     <x:row r="335" spans="1:11" outlineLevel="3">
@@ -7967,23 +7965,23 @@
         <x:v>123</x:v>
       </x:c>
       <x:c r="C335" s="41">
-        <x:v>1150</x:v>
+        <x:v>1350</x:v>
       </x:c>
       <x:c r="D335" s="40"/>
       <x:c r="E335" s="42">
-        <x:v>34418</x:v>
+        <x:v>34732</x:v>
       </x:c>
       <x:c r="F335" s="42">
-        <x:v>34418</x:v>
+        <x:v>34732</x:v>
       </x:c>
       <x:c r="G335" s="43">
-        <x:v>7671.9</x:v>
+        <x:v>8939.6</x:v>
       </x:c>
       <x:c r="H335" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I335" s="43">
-        <x:v>7671.9</x:v>
+        <x:v>8939.6</x:v>
       </x:c>
     </x:row>
     <x:row r="336" spans="1:11" outlineLevel="1">
@@ -8083,25 +8081,25 @@
         <x:v>125</x:v>
       </x:c>
       <x:c r="C341" s="41">
-        <x:v>1202</x:v>
+        <x:v>1102</x:v>
       </x:c>
       <x:c r="D341" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E341" s="42">
-        <x:v>34613</x:v>
+        <x:v>33761</x:v>
       </x:c>
       <x:c r="F341" s="42">
-        <x:v>34613</x:v>
+        <x:v>33761</x:v>
       </x:c>
       <x:c r="G341" s="43">
-        <x:v>4205</x:v>
+        <x:v>2844</x:v>
       </x:c>
       <x:c r="H341" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I341" s="43">
-        <x:v>4205</x:v>
+        <x:v>2844</x:v>
       </x:c>
     </x:row>
     <x:row r="342" spans="1:11" outlineLevel="3">
@@ -8133,23 +8131,23 @@
         <x:v>125</x:v>
       </x:c>
       <x:c r="C343" s="41">
-        <x:v>1302</x:v>
+        <x:v>1202</x:v>
       </x:c>
       <x:c r="D343" s="40"/>
       <x:c r="E343" s="42">
-        <x:v>34715</x:v>
+        <x:v>34613</x:v>
       </x:c>
       <x:c r="F343" s="42">
-        <x:v>34715</x:v>
+        <x:v>34613</x:v>
       </x:c>
       <x:c r="G343" s="43">
-        <x:v>24485</x:v>
+        <x:v>4205</x:v>
       </x:c>
       <x:c r="H343" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I343" s="43">
-        <x:v>24485</x:v>
+        <x:v>4205</x:v>
       </x:c>
     </x:row>
     <x:row r="344" spans="1:11" outlineLevel="3">
@@ -8181,23 +8179,23 @@
         <x:v>125</x:v>
       </x:c>
       <x:c r="C345" s="41">
-        <x:v>1102</x:v>
+        <x:v>1302</x:v>
       </x:c>
       <x:c r="D345" s="40"/>
       <x:c r="E345" s="42">
-        <x:v>33761</x:v>
+        <x:v>34715</x:v>
       </x:c>
       <x:c r="F345" s="42">
-        <x:v>33761</x:v>
+        <x:v>34715</x:v>
       </x:c>
       <x:c r="G345" s="43">
-        <x:v>2844</x:v>
+        <x:v>24485</x:v>
       </x:c>
       <x:c r="H345" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I345" s="43">
-        <x:v>2844</x:v>
+        <x:v>24485</x:v>
       </x:c>
     </x:row>
     <x:row r="346" spans="1:11" outlineLevel="2">
@@ -8431,25 +8429,25 @@
         <x:v>129</x:v>
       </x:c>
       <x:c r="C358" s="41">
-        <x:v>1200</x:v>
+        <x:v>1100</x:v>
       </x:c>
       <x:c r="D358" s="40" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="E358" s="42">
-        <x:v>34597</x:v>
+        <x:v>32679</x:v>
       </x:c>
       <x:c r="F358" s="42">
-        <x:v>34597</x:v>
+        <x:v>32679</x:v>
       </x:c>
       <x:c r="G358" s="43">
-        <x:v>1827</x:v>
+        <x:v>6094.8</x:v>
       </x:c>
       <x:c r="H358" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I358" s="43">
-        <x:v>1827</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="359" spans="1:11" outlineLevel="3">
@@ -8457,23 +8455,23 @@
         <x:v>129</x:v>
       </x:c>
       <x:c r="C359" s="41">
-        <x:v>1300</x:v>
+        <x:v>1200</x:v>
       </x:c>
       <x:c r="D359" s="40"/>
       <x:c r="E359" s="42">
-        <x:v>34709</x:v>
+        <x:v>34597</x:v>
       </x:c>
       <x:c r="F359" s="42">
-        <x:v>34709</x:v>
+        <x:v>34597</x:v>
       </x:c>
       <x:c r="G359" s="43">
-        <x:v>52729.25</x:v>
+        <x:v>1827</x:v>
       </x:c>
       <x:c r="H359" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I359" s="43">
-        <x:v>52729.25</x:v>
+        <x:v>1827</x:v>
       </x:c>
     </x:row>
     <x:row r="360" spans="1:11" outlineLevel="3">
@@ -8481,23 +8479,23 @@
         <x:v>129</x:v>
       </x:c>
       <x:c r="C360" s="41">
-        <x:v>1100</x:v>
+        <x:v>1300</x:v>
       </x:c>
       <x:c r="D360" s="40"/>
       <x:c r="E360" s="42">
-        <x:v>32679</x:v>
+        <x:v>34709</x:v>
       </x:c>
       <x:c r="F360" s="42">
-        <x:v>32679</x:v>
+        <x:v>34709</x:v>
       </x:c>
       <x:c r="G360" s="43">
-        <x:v>6094.8</x:v>
+        <x:v>52729.25</x:v>
       </x:c>
       <x:c r="H360" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I360" s="43">
-        <x:v>0</x:v>
+        <x:v>52729.25</x:v>
       </x:c>
     </x:row>
     <x:row r="361" spans="1:11" outlineLevel="2">
@@ -8519,25 +8517,25 @@
         <x:v>129</x:v>
       </x:c>
       <x:c r="C362" s="41">
-        <x:v>1127</x:v>
+        <x:v>1007</x:v>
       </x:c>
       <x:c r="D362" s="40" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="E362" s="42">
-        <x:v>34244</x:v>
+        <x:v>32265</x:v>
       </x:c>
       <x:c r="F362" s="42">
-        <x:v>34244</x:v>
+        <x:v>32264</x:v>
       </x:c>
       <x:c r="G362" s="43">
-        <x:v>25071</x:v>
+        <x:v>6500</x:v>
       </x:c>
       <x:c r="H362" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I362" s="43">
-        <x:v>25071</x:v>
+        <x:v>6500</x:v>
       </x:c>
     </x:row>
     <x:row r="363" spans="1:11" outlineLevel="3">
@@ -8545,23 +8543,23 @@
         <x:v>129</x:v>
       </x:c>
       <x:c r="C363" s="41">
-        <x:v>1207</x:v>
+        <x:v>1027</x:v>
       </x:c>
       <x:c r="D363" s="40"/>
       <x:c r="E363" s="42">
-        <x:v>34649</x:v>
+        <x:v>32332</x:v>
       </x:c>
       <x:c r="F363" s="42">
-        <x:v>34649</x:v>
+        <x:v>32331</x:v>
       </x:c>
       <x:c r="G363" s="43">
-        <x:v>12949.7</x:v>
+        <x:v>25210</x:v>
       </x:c>
       <x:c r="H363" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I363" s="43">
-        <x:v>12949.7</x:v>
+        <x:v>25210</x:v>
       </x:c>
     </x:row>
     <x:row r="364" spans="1:11" outlineLevel="3">
@@ -8569,23 +8567,23 @@
         <x:v>129</x:v>
       </x:c>
       <x:c r="C364" s="41">
-        <x:v>1027</x:v>
+        <x:v>1107</x:v>
       </x:c>
       <x:c r="D364" s="40"/>
       <x:c r="E364" s="42">
-        <x:v>32332</x:v>
+        <x:v>33901</x:v>
       </x:c>
       <x:c r="F364" s="42">
-        <x:v>32331</x:v>
+        <x:v>33901</x:v>
       </x:c>
       <x:c r="G364" s="43">
-        <x:v>25210</x:v>
+        <x:v>28389</x:v>
       </x:c>
       <x:c r="H364" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I364" s="43">
-        <x:v>25210</x:v>
+        <x:v>28389</x:v>
       </x:c>
     </x:row>
     <x:row r="365" spans="1:11" outlineLevel="3">
@@ -8593,23 +8591,23 @@
         <x:v>129</x:v>
       </x:c>
       <x:c r="C365" s="41">
-        <x:v>1107</x:v>
+        <x:v>1127</x:v>
       </x:c>
       <x:c r="D365" s="40"/>
       <x:c r="E365" s="42">
-        <x:v>33901</x:v>
+        <x:v>34244</x:v>
       </x:c>
       <x:c r="F365" s="42">
-        <x:v>33901</x:v>
+        <x:v>34244</x:v>
       </x:c>
       <x:c r="G365" s="43">
-        <x:v>28389</x:v>
+        <x:v>25071</x:v>
       </x:c>
       <x:c r="H365" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I365" s="43">
-        <x:v>28389</x:v>
+        <x:v>25071</x:v>
       </x:c>
     </x:row>
     <x:row r="366" spans="1:11" outlineLevel="3">
@@ -8617,23 +8615,23 @@
         <x:v>129</x:v>
       </x:c>
       <x:c r="C366" s="41">
-        <x:v>1007</x:v>
+        <x:v>1207</x:v>
       </x:c>
       <x:c r="D366" s="40"/>
       <x:c r="E366" s="42">
-        <x:v>32265</x:v>
+        <x:v>34649</x:v>
       </x:c>
       <x:c r="F366" s="42">
-        <x:v>32264</x:v>
+        <x:v>34649</x:v>
       </x:c>
       <x:c r="G366" s="43">
-        <x:v>6500</x:v>
+        <x:v>12949.7</x:v>
       </x:c>
       <x:c r="H366" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I366" s="43">
-        <x:v>6500</x:v>
+        <x:v>12949.7</x:v>
       </x:c>
     </x:row>
     <x:row r="367" spans="1:11" outlineLevel="1">
@@ -8669,25 +8667,25 @@
         <x:v>131</x:v>
       </x:c>
       <x:c r="C369" s="41">
-        <x:v>1140</x:v>
+        <x:v>1040</x:v>
       </x:c>
       <x:c r="D369" s="40" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="E369" s="42">
-        <x:v>34315</x:v>
+        <x:v>32391</x:v>
       </x:c>
       <x:c r="F369" s="42">
-        <x:v>34315</x:v>
+        <x:v>32390</x:v>
       </x:c>
       <x:c r="G369" s="43">
-        <x:v>1240</x:v>
+        <x:v>3632</x:v>
       </x:c>
       <x:c r="H369" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I369" s="43">
-        <x:v>1240</x:v>
+        <x:v>3632</x:v>
       </x:c>
     </x:row>
     <x:row r="370" spans="1:11" outlineLevel="3">
@@ -8695,23 +8693,23 @@
         <x:v>131</x:v>
       </x:c>
       <x:c r="C370" s="41">
-        <x:v>1040</x:v>
+        <x:v>1140</x:v>
       </x:c>
       <x:c r="D370" s="40"/>
       <x:c r="E370" s="42">
-        <x:v>32391</x:v>
+        <x:v>34315</x:v>
       </x:c>
       <x:c r="F370" s="42">
-        <x:v>32390</x:v>
+        <x:v>34315</x:v>
       </x:c>
       <x:c r="G370" s="43">
-        <x:v>3632</x:v>
+        <x:v>1240</x:v>
       </x:c>
       <x:c r="H370" s="43">
         <x:v>0</x:v>
       </x:c>
       <x:c r="I370" s="43">
-        <x:v>3632</x:v>
+        <x:v>1240</x:v>
       </x:c>
     </x:row>
     <x:row r="371" spans="1:11">

</xml_diff>